<commit_message>
Update Leave Card 3/15/2023 4:27 PM
</commit_message>
<xml_diff>
--- a/REGULAR/OJT/ARCILLA, MAYETTE A..xlsx
+++ b/REGULAR/OJT/ARCILLA, MAYETTE A..xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\REGULAR\OJT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CB3B71-E6F4-4DB9-B139-0C65FA3C2DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECB1B37-FC35-43B0-9A2E-13AF40C9E1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>PERIOD</t>
   </si>
@@ -2992,7 +2992,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3576" topLeftCell="A44" activePane="bottomLeft"/>
       <selection activeCell="F3" sqref="F3:G3"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3151,7 +3151,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>38.75</v>
+        <v>40</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3161,7 +3161,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>52.75</v>
+        <v>54</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -4203,13 +4203,15 @@
         <v>44958</v>
       </c>
       <c r="B59" s="20"/>
-      <c r="C59" s="13"/>
+      <c r="C59" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D59" s="39"/>
       <c r="E59" s="9"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G59" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H59" s="39"/>
       <c r="I59" s="9"/>
@@ -4220,7 +4222,9 @@
       <c r="A60" s="40">
         <v>44986</v>
       </c>
-      <c r="B60" s="20"/>
+      <c r="B60" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C60" s="13"/>
       <c r="D60" s="39"/>
       <c r="E60" s="9"/>
@@ -4232,7 +4236,9 @@
       <c r="H60" s="39"/>
       <c r="I60" s="9"/>
       <c r="J60" s="11"/>
-      <c r="K60" s="20"/>
+      <c r="K60" s="49">
+        <v>44988</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">

</xml_diff>